<commit_message>
Update lại bảng phân công tuần 6
</commit_message>
<xml_diff>
--- a/DoAn2/TaskManage.xlsx
+++ b/DoAn2/TaskManage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TaiLieuHoc\Nam 4\DoAn2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442140F7-156B-40D3-A918-A73FF0AE8F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD32984F-634E-40E3-99F7-ED45C79DCAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskManagement" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
   <si>
     <t>STT</t>
   </si>
@@ -183,6 +183,18 @@
   </si>
   <si>
     <t>Vẽ CSDL</t>
+  </si>
+  <si>
+    <t>Viết code xử lý dữ liệu bảng sinh viên</t>
+  </si>
+  <si>
+    <t>Viết code xử lý dữ liệu bảng Lớp</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện người dùng</t>
+  </si>
+  <si>
+    <t>Viết mô tả usecase</t>
   </si>
 </sst>
 </file>
@@ -421,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -543,11 +555,26 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="17">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -737,9 +764,9 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>7620</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>13</xdr:col>
@@ -787,9 +814,9 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>22</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>7620</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>23</xdr:col>
@@ -839,11 +866,11 @@
           <xdr:col>17</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>17</xdr:col>
-          <xdr:colOff>638175</xdr:colOff>
+          <xdr:colOff>640080</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1154,23 +1181,23 @@
       <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" style="7" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="38" width="5.7109375" style="5" customWidth="1"/>
-    <col min="39" max="16384" width="9.140625" style="5"/>
+    <col min="2" max="2" width="38.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="38" width="5.6640625" style="5" customWidth="1"/>
+    <col min="39" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>7</v>
       </c>
@@ -1207,7 +1234,7 @@
       <c r="V1" s="34"/>
       <c r="W1" s="6"/>
     </row>
-    <row r="2" spans="1:38" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>11</v>
       </c>
@@ -1354,7 +1381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28"/>
       <c r="B3" s="30"/>
       <c r="C3" s="28"/>
@@ -1487,7 +1514,7 @@
         <v>44852</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A4" s="16">
         <f>IF(B4="","",COUNTA($B$2:B4)-1)</f>
         <v>1</v>
@@ -1512,7 +1539,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A5" s="16">
         <f>IF(B5="","",COUNTA($B$2:B5)-1)</f>
         <v>2</v>
@@ -1537,7 +1564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A6" s="16">
         <f>IF(B6="","",COUNTA($B$2:B6)-1)</f>
         <v>3</v>
@@ -1562,7 +1589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A7" s="16">
         <f>IF(B7="","",COUNTA($B$2:B7)-1)</f>
         <v>4</v>
@@ -1587,7 +1614,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A8" s="16">
         <f>IF(B8="","",COUNTA($B$2:B8)-1)</f>
         <v>5</v>
@@ -1596,7 +1623,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="19">
         <v>44831</v>
@@ -1612,7 +1639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A9" s="16">
         <f>IF(B9="","",COUNTA($B$2:B9)-1)</f>
         <v>6</v>
@@ -1637,7 +1664,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A10" s="16">
         <f>IF(B10="","",COUNTA($B$2:B10)-1)</f>
         <v>7</v>
@@ -1649,20 +1676,20 @@
         <v>35</v>
       </c>
       <c r="D10" s="19">
-        <v>44832</v>
+        <v>44836</v>
       </c>
       <c r="E10" s="17">
         <v>3</v>
       </c>
       <c r="F10" s="21">
-        <f t="shared" si="2"/>
-        <v>44834</v>
+        <f>IF(D10="","",D10+E10-1)</f>
+        <v>44838</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A11" s="16">
         <f>IF(B11="","",COUNTA($B$2:B11)-1)</f>
         <v>8</v>
@@ -1671,23 +1698,23 @@
         <v>43</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D11" s="19">
-        <v>44833</v>
+        <v>44837</v>
       </c>
       <c r="E11" s="17">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F11" s="21">
         <f t="shared" si="2"/>
-        <v>44834</v>
+        <v>44843</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A12" s="16">
         <f>IF(B12="","",COUNTA($B$2:B12)-1)</f>
         <v>9</v>
@@ -1696,68 +1723,98 @@
         <v>44</v>
       </c>
       <c r="C12" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="19">
+        <v>44843</v>
+      </c>
+      <c r="E12" s="17">
+        <v>10</v>
+      </c>
+      <c r="F12" s="21">
+        <f t="shared" si="2"/>
+        <v>44852</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A13" s="16">
+        <f>IF(B13="","",COUNTA($B$2:B13)-1)</f>
+        <v>10</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="19">
+        <v>44839</v>
+      </c>
+      <c r="E13" s="17">
+        <v>6</v>
+      </c>
+      <c r="F13" s="21">
+        <f t="shared" si="2"/>
+        <v>44844</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A14" s="16">
+        <f>IF(B14="","",COUNTA($B$2:B14)-1)</f>
+        <v>11</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="19">
-        <v>44834</v>
-      </c>
-      <c r="E12" s="17">
+      <c r="D14" s="19">
+        <v>44842</v>
+      </c>
+      <c r="E14" s="17">
         <v>5</v>
       </c>
-      <c r="F12" s="21">
-        <f t="shared" si="2"/>
-        <v>44838</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="str">
-        <f>IF(B13="","",COUNTA($B$2:B13)-1)</f>
-        <v/>
-      </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="21" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G13" s="17"/>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="str">
-        <f>IF(B14="","",COUNTA($B$2:B14)-1)</f>
-        <v/>
-      </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="21" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G14" s="17"/>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="str">
+      <c r="F14" s="21">
+        <f t="shared" si="2"/>
+        <v>44846</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A15" s="16">
         <f>IF(B15="","",COUNTA($B$2:B15)-1)</f>
-        <v/>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="21" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="19">
+        <v>44844</v>
+      </c>
+      <c r="E15" s="17">
+        <v>5</v>
+      </c>
+      <c r="F15" s="21">
+        <f t="shared" si="2"/>
+        <v>44848</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="str">
         <f>IF(B16="","",COUNTA($B$2:B16)-1)</f>
         <v/>
@@ -1772,7 +1829,7 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="str">
         <f>IF(B17="","",COUNTA($B$2:B17)-1)</f>
         <v/>
@@ -1787,7 +1844,7 @@
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="str">
         <f>IF(B18="","",COUNTA($B$2:B18)-1)</f>
         <v/>
@@ -1802,7 +1859,7 @@
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="str">
         <f>IF(B19="","",COUNTA($B$2:B19)-1)</f>
         <v/>
@@ -1817,7 +1874,7 @@
       </c>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="str">
         <f>IF(B20="","",COUNTA($B$2:B20)-1)</f>
         <v/>
@@ -1832,7 +1889,7 @@
       </c>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="16" t="str">
         <f>IF(B21="","",COUNTA($B$2:B21)-1)</f>
         <v/>
@@ -1847,7 +1904,7 @@
       </c>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="str">
         <f>IF(B22="","",COUNTA($B$2:B22)-1)</f>
         <v/>
@@ -1862,7 +1919,7 @@
       </c>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="str">
         <f>IF(B23="","",COUNTA($B$2:B23)-1)</f>
         <v/>
@@ -1877,7 +1934,7 @@
       </c>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="str">
         <f>IF(B24="","",COUNTA($B$2:B24)-1)</f>
         <v/>
@@ -1892,7 +1949,7 @@
       </c>
       <c r="G24" s="17"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="16" t="str">
         <f>IF(B25="","",COUNTA($B$2:B25)-1)</f>
         <v/>
@@ -1907,7 +1964,7 @@
       </c>
       <c r="G25" s="17"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="str">
         <f>IF(B26="","",COUNTA($B$2:B26)-1)</f>
         <v/>
@@ -1922,7 +1979,7 @@
       </c>
       <c r="G26" s="17"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="str">
         <f>IF(B27="","",COUNTA($B$2:B27)-1)</f>
         <v/>
@@ -1937,7 +1994,7 @@
       </c>
       <c r="G27" s="17"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="16" t="str">
         <f>IF(B28="","",COUNTA($B$2:B28)-1)</f>
         <v/>
@@ -1952,7 +2009,7 @@
       </c>
       <c r="G28" s="17"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="16" t="str">
         <f>IF(B29="","",COUNTA($B$2:B29)-1)</f>
         <v/>
@@ -1967,7 +2024,7 @@
       </c>
       <c r="G29" s="17"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="16" t="str">
         <f>IF(B30="","",COUNTA($B$2:B30)-1)</f>
         <v/>
@@ -1982,7 +2039,7 @@
       </c>
       <c r="G30" s="17"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="16" t="str">
         <f>IF(B31="","",COUNTA($B$2:B31)-1)</f>
         <v/>
@@ -1997,7 +2054,7 @@
       </c>
       <c r="G31" s="17"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="16" t="str">
         <f>IF(B32="","",COUNTA($B$2:B32)-1)</f>
         <v/>
@@ -2012,7 +2069,7 @@
       </c>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="16" t="str">
         <f>IF(B33="","",COUNTA($B$2:B33)-1)</f>
         <v/>
@@ -2027,7 +2084,7 @@
       </c>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="16" t="str">
         <f>IF(B34="","",COUNTA($B$2:B34)-1)</f>
         <v/>
@@ -2042,7 +2099,7 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="16" t="str">
         <f>IF(B35="","",COUNTA($B$2:B35)-1)</f>
         <v/>
@@ -2057,7 +2114,7 @@
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="str">
         <f>IF(B36="","",COUNTA($B$2:B36)-1)</f>
         <v/>
@@ -2072,7 +2129,7 @@
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="16" t="str">
         <f>IF(B37="","",COUNTA($B$2:B37)-1)</f>
         <v/>
@@ -2087,7 +2144,7 @@
       </c>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="16" t="str">
         <f>IF(B38="","",COUNTA($B$2:B38)-1)</f>
         <v/>
@@ -2102,7 +2159,7 @@
       </c>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="str">
         <f>IF(B39="","",COUNTA($B$2:B39)-1)</f>
         <v/>
@@ -2117,7 +2174,7 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="16" t="str">
         <f>IF(B40="","",COUNTA($B$2:B40)-1)</f>
         <v/>
@@ -2132,7 +2189,7 @@
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="16" t="str">
         <f>IF(B41="","",COUNTA($B$2:B41)-1)</f>
         <v/>
@@ -2147,7 +2204,7 @@
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="16" t="str">
         <f>IF(B42="","",COUNTA($B$2:B42)-1)</f>
         <v/>
@@ -2162,7 +2219,7 @@
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="16" t="str">
         <f>IF(B43="","",COUNTA($B$2:B43)-1)</f>
         <v/>
@@ -2177,7 +2234,7 @@
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="str">
         <f>IF(B44="","",COUNTA($B$2:B44)-1)</f>
         <v/>
@@ -2192,7 +2249,7 @@
       </c>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="16" t="str">
         <f>IF(B45="","",COUNTA($B$2:B45)-1)</f>
         <v/>
@@ -2207,7 +2264,7 @@
       </c>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="16" t="str">
         <f>IF(B46="","",COUNTA($B$2:B46)-1)</f>
         <v/>
@@ -2222,7 +2279,7 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="16" t="str">
         <f>IF(B47="","",COUNTA($B$2:B47)-1)</f>
         <v/>
@@ -2237,7 +2294,7 @@
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="str">
         <f>IF(B48="","",COUNTA($B$2:B48)-1)</f>
         <v/>
@@ -2252,7 +2309,7 @@
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="16" t="str">
         <f>IF(B49="","",COUNTA($B$2:B49)-1)</f>
         <v/>
@@ -2267,7 +2324,7 @@
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="16" t="str">
         <f>IF(B50="","",COUNTA($B$2:B50)-1)</f>
         <v/>
@@ -2302,58 +2359,58 @@
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="H3:AL3">
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="16" priority="4">
       <formula>AND(H$3=TODAY(),$A4&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="18">
+    <cfRule type="expression" dxfId="15" priority="18">
       <formula>DAY(H$3)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:AL3">
-    <cfRule type="expression" dxfId="13" priority="17">
+    <cfRule type="expression" dxfId="14" priority="17">
       <formula>WEEKDAY(H$3)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:AL50">
-    <cfRule type="expression" dxfId="12" priority="12">
+    <cfRule type="expression" dxfId="13" priority="12">
       <formula>AND(H$3&gt;=$D4,H$3&lt;=$F4,$G4="Tạm dừng")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>AND(H$3&gt;=$D4,H$3&lt;=$F4,$G4="Chưa thực hiện")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="14">
+    <cfRule type="expression" dxfId="11" priority="14">
       <formula>AND(H$3&gt;=$D4,H$3&lt;=$F4,$G4="Đã hoàn thành")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="15">
+    <cfRule type="expression" dxfId="10" priority="15">
       <formula>AND(H$3&gt;=$D4,H$3&lt;=$F4,$G4="Đang thực hiện")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:AL50">
-    <cfRule type="expression" dxfId="8" priority="11">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>$A4&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:G50">
-    <cfRule type="expression" dxfId="7" priority="10">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>$A4&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A50">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>$G4="Tạm dừng"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>$G4="Đã hoàn thành"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>$G4="Đang thực hiện"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>$G4="Chưa thực hiện"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:AL6 Z7:Z50 U7:U18">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>AND(H$3=TODAY(),$A4&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2371,9 +2428,9 @@
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>12</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>7620</xdr:colOff>
                     <xdr:row>0</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>13</xdr:col>
@@ -2393,9 +2450,9 @@
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>22</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>7620</xdr:colOff>
                     <xdr:row>0</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>7620</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>23</xdr:col>
@@ -2417,11 +2474,11 @@
                     <xdr:col>17</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>0</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>17</xdr:col>
-                    <xdr:colOff>638175</xdr:colOff>
+                    <xdr:colOff>640080</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -2435,7 +2492,7 @@
   </mc:AlternateContent>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{58AF4E67-B6DE-457D-96D9-4B8B56E6D807}">
           <x14:formula1>
             <xm:f>List!$C$6:$C$12</xm:f>
@@ -2464,13 +2521,19 @@
           <x14:formula1>
             <xm:f>List!$H$3:$H$10</xm:f>
           </x14:formula1>
-          <xm:sqref>B7:B8 B9:B10 B15:B50</xm:sqref>
+          <xm:sqref>B7:B8 B9:B10 B16:B50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BC71BFD7-A4C2-4799-ADCA-E520354EAD25}">
           <x14:formula1>
-            <xm:f>List!$H$3:$H$13</xm:f>
+            <xm:f>List!$H$3:$H$15</xm:f>
           </x14:formula1>
-          <xm:sqref>B11:B14</xm:sqref>
+          <xm:sqref>B11:B12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A7EB8BD3-F8DF-4532-BC8C-3D1AA3DC218C}">
+          <x14:formula1>
+            <xm:f>List!$H$3:$H$20</xm:f>
+          </x14:formula1>
+          <xm:sqref>B13 B14 B15</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2483,23 +2546,23 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="1"/>
+    <col min="5" max="5" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
         <v>17</v>
       </c>
@@ -2514,7 +2577,7 @@
       </c>
       <c r="H1" s="36"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -2534,7 +2597,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <f>IF(C3="","",COUNTA($C$2:C3)-1)</f>
         <v>1</v>
@@ -2556,7 +2619,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <f>IF(C4="","",COUNTA($C$2:C4)-1)</f>
         <v>2</v>
@@ -2578,7 +2641,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <f>IF(C5="","",COUNTA($C$2:C5)-1)</f>
         <v>3</v>
@@ -2600,7 +2663,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <f>IF(C6="","",COUNTA($C$2:C6)-1)</f>
         <v>4</v>
@@ -2618,7 +2681,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <f>IF(C7="","",COUNTA($C$2:C7)-1)</f>
         <v>5</v>
@@ -2636,7 +2699,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <f>IF(C8="","",COUNTA($C$2:C8)-1)</f>
         <v>6</v>
@@ -2654,7 +2717,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <f>IF(C9="","",COUNTA($C$2:C9)-1)</f>
         <v>7</v>
@@ -2672,7 +2735,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <f>IF(C10="","",COUNTA($C$2:C10)-1)</f>
         <v>8</v>
@@ -2690,7 +2753,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <f>IF(C11="","",COUNTA($C$2:C11)-1)</f>
         <v>9</v>
@@ -2707,7 +2770,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <f>IF(C12="","",COUNTA($C$2:C12)-1)</f>
         <v>10</v>
@@ -2724,266 +2787,274 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G13" s="13" t="str">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G13" s="13">
         <f>IF(H13="","",COUNTA($H$2:H13)-1)</f>
-        <v/>
-      </c>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G14" s="13" t="str">
+        <v>11</v>
+      </c>
+      <c r="H13" s="37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G14" s="13">
         <f>IF(H14="","",COUNTA($H$2:H14)-1)</f>
-        <v/>
-      </c>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G15" s="13" t="str">
+        <v>12</v>
+      </c>
+      <c r="H14" s="37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G15" s="13">
         <f>IF(H15="","",COUNTA($H$2:H15)-1)</f>
-        <v/>
-      </c>
-      <c r="H15" s="13"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G16" s="13" t="str">
+        <v>13</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G16" s="13">
         <f>IF(H16="","",COUNTA($H$2:H16)-1)</f>
-        <v/>
-      </c>
-      <c r="H16" s="13"/>
-    </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G17" s="13" t="str">
         <f>IF(H17="","",COUNTA($H$2:H17)-1)</f>
         <v/>
       </c>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G18" s="13" t="str">
         <f>IF(H18="","",COUNTA($H$2:H18)-1)</f>
         <v/>
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G19" s="13" t="str">
         <f>IF(H19="","",COUNTA($H$2:H19)-1)</f>
         <v/>
       </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G20" s="13" t="str">
         <f>IF(H20="","",COUNTA($H$2:H20)-1)</f>
         <v/>
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G21" s="13" t="str">
         <f>IF(H21="","",COUNTA($H$2:H21)-1)</f>
         <v/>
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G22" s="13" t="str">
         <f>IF(H22="","",COUNTA($H$2:H22)-1)</f>
         <v/>
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G23" s="13" t="str">
         <f>IF(H23="","",COUNTA($H$2:H23)-1)</f>
         <v/>
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G24" s="13" t="str">
         <f>IF(H24="","",COUNTA($H$2:H24)-1)</f>
         <v/>
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G25" s="13" t="str">
         <f>IF(H25="","",COUNTA($H$2:H25)-1)</f>
         <v/>
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G26" s="13" t="str">
         <f>IF(H26="","",COUNTA($H$2:H26)-1)</f>
         <v/>
       </c>
       <c r="H26" s="13"/>
     </row>
-    <row r="27" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G27" s="13" t="str">
         <f>IF(H27="","",COUNTA($H$2:H27)-1)</f>
         <v/>
       </c>
       <c r="H27" s="13"/>
     </row>
-    <row r="28" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G28" s="13" t="str">
         <f>IF(H28="","",COUNTA($H$2:H28)-1)</f>
         <v/>
       </c>
       <c r="H28" s="13"/>
     </row>
-    <row r="29" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G29" s="13" t="str">
         <f>IF(H29="","",COUNTA($H$2:H29)-1)</f>
         <v/>
       </c>
       <c r="H29" s="13"/>
     </row>
-    <row r="30" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G30" s="13" t="str">
         <f>IF(H30="","",COUNTA($H$2:H30)-1)</f>
         <v/>
       </c>
       <c r="H30" s="13"/>
     </row>
-    <row r="31" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G31" s="13" t="str">
         <f>IF(H31="","",COUNTA($H$2:H31)-1)</f>
         <v/>
       </c>
       <c r="H31" s="13"/>
     </row>
-    <row r="32" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G32" s="13" t="str">
         <f>IF(H32="","",COUNTA($H$2:H32)-1)</f>
         <v/>
       </c>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G33" s="13" t="str">
         <f>IF(H33="","",COUNTA($H$2:H33)-1)</f>
         <v/>
       </c>
       <c r="H33" s="13"/>
     </row>
-    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G34" s="13" t="str">
         <f>IF(H34="","",COUNTA($H$2:H34)-1)</f>
         <v/>
       </c>
       <c r="H34" s="13"/>
     </row>
-    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G35" s="13" t="str">
         <f>IF(H35="","",COUNTA($H$2:H35)-1)</f>
         <v/>
       </c>
       <c r="H35" s="13"/>
     </row>
-    <row r="36" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G36" s="13" t="str">
         <f>IF(H36="","",COUNTA($H$2:H36)-1)</f>
         <v/>
       </c>
       <c r="H36" s="13"/>
     </row>
-    <row r="37" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G37" s="13" t="str">
         <f>IF(H37="","",COUNTA($H$2:H37)-1)</f>
         <v/>
       </c>
       <c r="H37" s="13"/>
     </row>
-    <row r="38" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G38" s="13" t="str">
         <f>IF(H38="","",COUNTA($H$2:H38)-1)</f>
         <v/>
       </c>
       <c r="H38" s="13"/>
     </row>
-    <row r="39" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G39" s="13" t="str">
         <f>IF(H39="","",COUNTA($H$2:H39)-1)</f>
         <v/>
       </c>
       <c r="H39" s="13"/>
     </row>
-    <row r="40" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G40" s="13" t="str">
         <f>IF(H40="","",COUNTA($H$2:H40)-1)</f>
         <v/>
       </c>
       <c r="H40" s="13"/>
     </row>
-    <row r="41" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G41" s="13" t="str">
         <f>IF(H41="","",COUNTA($H$2:H41)-1)</f>
         <v/>
       </c>
       <c r="H41" s="13"/>
     </row>
-    <row r="42" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G42" s="13" t="str">
         <f>IF(H42="","",COUNTA($H$2:H42)-1)</f>
         <v/>
       </c>
       <c r="H42" s="13"/>
     </row>
-    <row r="43" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G43" s="13" t="str">
         <f>IF(H43="","",COUNTA($H$2:H43)-1)</f>
         <v/>
       </c>
       <c r="H43" s="13"/>
     </row>
-    <row r="44" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G44" s="13" t="str">
         <f>IF(H44="","",COUNTA($H$2:H44)-1)</f>
         <v/>
       </c>
       <c r="H44" s="13"/>
     </row>
-    <row r="45" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G45" s="13" t="str">
         <f>IF(H45="","",COUNTA($H$2:H45)-1)</f>
         <v/>
       </c>
       <c r="H45" s="13"/>
     </row>
-    <row r="46" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G46" s="13" t="str">
         <f>IF(H46="","",COUNTA($H$2:H46)-1)</f>
         <v/>
       </c>
       <c r="H46" s="13"/>
     </row>
-    <row r="47" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G47" s="13" t="str">
         <f>IF(H47="","",COUNTA($H$2:H47)-1)</f>
         <v/>
       </c>
       <c r="H47" s="13"/>
     </row>
-    <row r="48" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G48" s="13" t="str">
         <f>IF(H48="","",COUNTA($H$2:H48)-1)</f>
         <v/>
       </c>
       <c r="H48" s="13"/>
     </row>
-    <row r="49" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G49" s="13" t="str">
         <f>IF(H49="","",COUNTA($H$2:H49)-1)</f>
         <v/>
       </c>
       <c r="H49" s="13"/>
     </row>
-    <row r="50" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G50" s="13" t="str">
         <f>IF(H50="","",COUNTA($H$2:H50)-1)</f>
         <v/>
@@ -2996,13 +3067,18 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:C12">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:H50">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="G3:H3 G20:H50 H16:H19 H4:H12 G4:G19">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$G3&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15:H16">
+    <cfRule type="expression" dxfId="0" priority="20">
+      <formula>$G13&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>